<commit_message>
Finished command focus time and threshold tests
</commit_message>
<xml_diff>
--- a/praca/badania/badanie2.xlsx
+++ b/praca/badania/badanie2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abani\Desktop\Praca magisterska\praca\badania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA81AAFF-9CF5-4D39-8DA6-BB511735DB50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD5A54C-9810-48DE-8068-DDAB08DC7D74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,12 +105,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -630,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -641,11 +650,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,62 +715,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -994,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:AH56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12:AH21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,21 +1026,21 @@
     </row>
     <row r="8" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="12"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="42"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
         <v>1</v>
@@ -1042,7 +1054,7 @@
       <c r="U9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB9" s="30" t="s">
+      <c r="AB9" s="28" t="s">
         <v>21</v>
       </c>
       <c r="AC9" s="29"/>
@@ -1050,30 +1062,30 @@
       <c r="AE9" s="29"/>
       <c r="AF9" s="29"/>
       <c r="AG9" s="29"/>
-      <c r="AH9" s="31"/>
+      <c r="AH9" s="30"/>
     </row>
     <row r="10" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="13" t="s">
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="13" t="s">
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
       <c r="Q10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1089,24 +1101,24 @@
       <c r="U10" s="2">
         <v>5</v>
       </c>
-      <c r="AB10" s="20" t="s">
+      <c r="AB10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AC10" s="16" t="s">
+      <c r="AC10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="17" t="s">
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="16" t="s">
+      <c r="AF10" s="34"/>
+      <c r="AG10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="18"/>
+      <c r="AH10" s="34"/>
     </row>
     <row r="11" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="27"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="5" t="s">
         <v>1</v>
       </c>
@@ -1143,26 +1155,26 @@
       <c r="O11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="40" t="s">
+      <c r="Q11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="R11" s="40"/>
-      <c r="S11" s="40"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="40"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AB11" s="27"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AB11" s="32"/>
       <c r="AC11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AE11" s="28" t="s">
+      <c r="AE11" s="15" t="s">
         <v>19</v>
       </c>
       <c r="AF11" s="6" t="s">
@@ -1176,85 +1188,85 @@
       </c>
     </row>
     <row r="12" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C12" s="23">
+      <c r="C12" s="11">
         <v>0.1</v>
       </c>
-      <c r="D12" s="24">
-        <v>10</v>
-      </c>
-      <c r="E12" s="25">
-        <v>0</v>
-      </c>
-      <c r="F12" s="25">
-        <v>10</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0</v>
-      </c>
-      <c r="H12" s="24">
-        <v>10</v>
-      </c>
-      <c r="I12" s="25">
-        <v>0</v>
-      </c>
-      <c r="J12" s="25">
-        <v>10</v>
-      </c>
-      <c r="K12" s="26">
-        <v>0</v>
-      </c>
-      <c r="L12" s="24">
-        <v>10</v>
-      </c>
-      <c r="M12" s="25">
-        <v>0</v>
-      </c>
-      <c r="N12" s="25">
-        <v>10</v>
-      </c>
-      <c r="O12" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AB12" s="23">
+      <c r="D12" s="12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>10</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>10</v>
+      </c>
+      <c r="K12" s="14">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>10</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <v>10</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AB12" s="11">
         <v>0.1</v>
       </c>
-      <c r="AC12" s="32">
+      <c r="AC12" s="16">
         <f>D12/10</f>
         <v>1</v>
       </c>
-      <c r="AD12" s="34">
+      <c r="AD12" s="18">
         <f>F12/10</f>
         <v>1</v>
       </c>
-      <c r="AE12" s="35">
+      <c r="AE12" s="19">
         <f>H12/10</f>
         <v>1</v>
       </c>
-      <c r="AF12" s="33">
+      <c r="AF12" s="17">
         <f>J12/10</f>
         <v>1</v>
       </c>
-      <c r="AG12" s="32">
+      <c r="AG12" s="16">
         <f>L12/10</f>
         <v>1</v>
       </c>
-      <c r="AH12" s="34">
+      <c r="AH12" s="18">
         <f>N12/10</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C13" s="21">
+      <c r="C13" s="9">
         <v>0.2</v>
       </c>
       <c r="D13" s="3">
@@ -1293,46 +1305,46 @@
       <c r="O13" s="4">
         <v>4</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AB13" s="21">
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36"/>
+      <c r="AB13" s="9">
         <v>0.2</v>
       </c>
-      <c r="AC13" s="32">
+      <c r="AC13" s="16">
         <f t="shared" ref="AC13:AC21" si="0">D13/10</f>
         <v>1</v>
       </c>
-      <c r="AD13" s="34">
+      <c r="AD13" s="18">
         <f t="shared" ref="AD13:AD21" si="1">F13/10</f>
         <v>1</v>
       </c>
-      <c r="AE13" s="35">
+      <c r="AE13" s="19">
         <f t="shared" ref="AE13:AE21" si="2">H13/10</f>
         <v>1</v>
       </c>
-      <c r="AF13" s="33">
+      <c r="AF13" s="17">
         <f t="shared" ref="AF13:AF21" si="3">J13/10</f>
         <v>1</v>
       </c>
-      <c r="AG13" s="32">
+      <c r="AG13" s="16">
         <f t="shared" ref="AG13:AG21" si="4">L13/10</f>
         <v>0.6</v>
       </c>
-      <c r="AH13" s="34">
+      <c r="AH13" s="18">
         <f t="shared" ref="AH13:AH21" si="5">N13/10</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C14" s="21">
+      <c r="C14" s="9">
         <v>0.3</v>
       </c>
       <c r="D14" s="3">
@@ -1371,46 +1383,46 @@
       <c r="O14" s="4">
         <v>4</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AB14" s="21">
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AB14" s="9">
         <v>0.3</v>
       </c>
-      <c r="AC14" s="32">
+      <c r="AC14" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AD14" s="34">
+      <c r="AD14" s="18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AE14" s="35">
+      <c r="AE14" s="19">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="AF14" s="33">
+      <c r="AF14" s="17">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="AG14" s="32">
+      <c r="AG14" s="16">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="AH14" s="34">
+      <c r="AH14" s="18">
         <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C15" s="21">
+      <c r="C15" s="9">
         <v>0.4</v>
       </c>
       <c r="D15" s="3">
@@ -1449,46 +1461,46 @@
       <c r="O15" s="4">
         <v>6</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AB15" s="21">
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+      <c r="AB15" s="9">
         <v>0.4</v>
       </c>
-      <c r="AC15" s="32">
+      <c r="AC15" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AD15" s="34">
+      <c r="AD15" s="18">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AE15" s="35">
+      <c r="AE15" s="19">
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="AF15" s="33">
+      <c r="AF15" s="17">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="AG15" s="32">
+      <c r="AG15" s="16">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="AH15" s="34">
+      <c r="AH15" s="18">
         <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C16" s="21">
+      <c r="C16" s="9">
         <v>0.5</v>
       </c>
       <c r="D16" s="3">
@@ -1506,10 +1518,10 @@
       <c r="H16" s="3">
         <v>1</v>
       </c>
-      <c r="I16" s="44">
+      <c r="I16" s="27">
         <v>9</v>
       </c>
-      <c r="J16" s="44">
+      <c r="J16" s="27">
         <v>0</v>
       </c>
       <c r="K16" s="4">
@@ -1527,46 +1539,46 @@
       <c r="O16" s="4">
         <v>10</v>
       </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AB16" s="21">
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AB16" s="9">
         <v>0.5</v>
       </c>
-      <c r="AC16" s="32">
+      <c r="AC16" s="16">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="AD16" s="34">
+      <c r="AD16" s="18">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AE16" s="35">
+      <c r="AE16" s="19">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="AF16" s="33">
+      <c r="AF16" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG16" s="32">
+      <c r="AG16" s="16">
         <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
-      <c r="AH16" s="34">
+      <c r="AH16" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C17" s="21">
+      <c r="C17" s="9">
         <v>0.6</v>
       </c>
       <c r="D17" s="3">
@@ -1581,7 +1593,7 @@
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="8">
         <v>0</v>
       </c>
       <c r="I17" s="2">
@@ -1590,7 +1602,7 @@
       <c r="J17" s="2">
         <v>0</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="25">
         <v>10</v>
       </c>
       <c r="L17" s="3">
@@ -1605,46 +1617,46 @@
       <c r="O17" s="4">
         <v>10</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AB17" s="21">
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AB17" s="9">
         <v>0.6</v>
       </c>
-      <c r="AC17" s="32">
+      <c r="AC17" s="16">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="AD17" s="34">
+      <c r="AD17" s="18">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AE17" s="35">
+      <c r="AE17" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF17" s="33">
+      <c r="AF17" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG17" s="32">
+      <c r="AG17" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH17" s="34">
+      <c r="AH17" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C18" s="21">
+      <c r="C18" s="9">
         <v>0.7</v>
       </c>
       <c r="D18" s="3">
@@ -1659,7 +1671,7 @@
       <c r="G18" s="4">
         <v>3</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="8">
         <v>0</v>
       </c>
       <c r="I18" s="2">
@@ -1668,7 +1680,7 @@
       <c r="J18" s="2">
         <v>0</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="25">
         <v>10</v>
       </c>
       <c r="L18" s="3">
@@ -1683,46 +1695,46 @@
       <c r="O18" s="4">
         <v>10</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AB18" s="21">
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AB18" s="9">
         <v>0.7</v>
       </c>
-      <c r="AC18" s="32">
+      <c r="AC18" s="16">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="AD18" s="34">
+      <c r="AD18" s="18">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="AE18" s="35">
+      <c r="AE18" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF18" s="33">
+      <c r="AF18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG18" s="32">
+      <c r="AG18" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH18" s="34">
+      <c r="AH18" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C19" s="21">
+      <c r="C19" s="9">
         <v>0.8</v>
       </c>
       <c r="D19" s="3">
@@ -1737,7 +1749,7 @@
       <c r="G19" s="4">
         <v>7</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="8">
         <v>0</v>
       </c>
       <c r="I19" s="2">
@@ -1746,7 +1758,7 @@
       <c r="J19" s="2">
         <v>0</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="25">
         <v>10</v>
       </c>
       <c r="L19" s="3">
@@ -1761,46 +1773,46 @@
       <c r="O19" s="4">
         <v>10</v>
       </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AB19" s="21">
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AB19" s="9">
         <v>0.8</v>
       </c>
-      <c r="AC19" s="32">
+      <c r="AC19" s="16">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="AD19" s="34">
+      <c r="AD19" s="18">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="AE19" s="35">
+      <c r="AE19" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF19" s="33">
+      <c r="AF19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG19" s="32">
+      <c r="AG19" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH19" s="34">
+      <c r="AH19" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C20" s="21">
+      <c r="C20" s="9">
         <v>0.9</v>
       </c>
       <c r="D20" s="3">
@@ -1815,7 +1827,7 @@
       <c r="G20" s="4">
         <v>10</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="8">
         <v>0</v>
       </c>
       <c r="I20" s="2">
@@ -1824,7 +1836,7 @@
       <c r="J20" s="2">
         <v>0</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="25">
         <v>10</v>
       </c>
       <c r="L20" s="3">
@@ -1839,46 +1851,46 @@
       <c r="O20" s="4">
         <v>10</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AB20" s="21">
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="36"/>
+      <c r="AB20" s="9">
         <v>0.9</v>
       </c>
-      <c r="AC20" s="32">
+      <c r="AC20" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD20" s="34">
+      <c r="AD20" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE20" s="35">
+      <c r="AE20" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF20" s="33">
+      <c r="AF20" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG20" s="32">
+      <c r="AG20" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH20" s="34">
+      <c r="AH20" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="22">
+      <c r="C21" s="10">
         <v>1</v>
       </c>
       <c r="D21" s="5">
@@ -1893,7 +1905,7 @@
       <c r="G21" s="7">
         <v>10</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H21" s="24">
         <v>0</v>
       </c>
       <c r="I21" s="6">
@@ -1902,7 +1914,7 @@
       <c r="J21" s="6">
         <v>0</v>
       </c>
-      <c r="K21" s="43">
+      <c r="K21" s="26">
         <v>10</v>
       </c>
       <c r="L21" s="5">
@@ -1917,73 +1929,73 @@
       <c r="O21" s="7">
         <v>10</v>
       </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AB21" s="22">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="36">
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
+      <c r="AB21" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD21" s="37">
+      <c r="AD21" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE21" s="38">
+      <c r="AE21" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF21" s="39">
+      <c r="AF21" s="23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG21" s="36">
+      <c r="AG21" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH21" s="37">
+      <c r="AH21" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
     </row>
     <row r="24" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="12"/>
+      <c r="C25" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="42"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2" t="s">
         <v>1</v>
@@ -1997,7 +2009,7 @@
       <c r="U25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB25" s="30" t="s">
+      <c r="AB25" s="28" t="s">
         <v>10</v>
       </c>
       <c r="AC25" s="29"/>
@@ -2005,30 +2017,30 @@
       <c r="AE25" s="29"/>
       <c r="AF25" s="29"/>
       <c r="AG25" s="29"/>
-      <c r="AH25" s="31"/>
+      <c r="AH25" s="30"/>
     </row>
     <row r="26" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="13" t="s">
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="13" t="s">
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="15"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39"/>
       <c r="Q26" s="2" t="s">
         <v>4</v>
       </c>
@@ -2044,24 +2056,24 @@
       <c r="U26" s="2">
         <v>5</v>
       </c>
-      <c r="AB26" s="20" t="s">
+      <c r="AB26" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AC26" s="16" t="s">
+      <c r="AC26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AD26" s="18"/>
-      <c r="AE26" s="17" t="s">
+      <c r="AD26" s="34"/>
+      <c r="AE26" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF26" s="18"/>
-      <c r="AG26" s="16" t="s">
+      <c r="AF26" s="34"/>
+      <c r="AG26" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AH26" s="18"/>
+      <c r="AH26" s="34"/>
     </row>
     <row r="27" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="27"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="5" t="s">
         <v>1</v>
       </c>
@@ -2098,14 +2110,14 @@
       <c r="O27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB27" s="27"/>
+      <c r="AB27" s="32"/>
       <c r="AC27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AD27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AE27" s="28" t="s">
+      <c r="AE27" s="15" t="s">
         <v>19</v>
       </c>
       <c r="AF27" s="6" t="s">
@@ -2119,89 +2131,89 @@
       </c>
     </row>
     <row r="28" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C28" s="23">
+      <c r="C28" s="11">
         <v>0.1</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="12">
         <v>5</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="13">
         <v>5</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="13">
         <v>3</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="13">
         <v>7</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="12">
         <v>5</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="13">
         <v>5</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="13">
         <v>2</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="13">
         <v>8</v>
       </c>
-      <c r="L28" s="24">
+      <c r="L28" s="12">
         <v>5</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="13">
         <v>5</v>
       </c>
-      <c r="N28" s="25">
-        <v>0</v>
-      </c>
-      <c r="O28" s="25">
-        <v>10</v>
-      </c>
-      <c r="Q28" s="9" t="s">
+      <c r="N28" s="13">
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9" t="s">
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
+      <c r="V28" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="W28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-      <c r="AB28" s="23">
+      <c r="W28" s="36"/>
+      <c r="X28" s="36"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="36"/>
+      <c r="AB28" s="11">
         <v>0.1</v>
       </c>
-      <c r="AC28" s="32">
+      <c r="AC28" s="16">
         <f>D28/10</f>
         <v>0.5</v>
       </c>
-      <c r="AD28" s="34">
+      <c r="AD28" s="18">
         <f>F28/10</f>
         <v>0.3</v>
       </c>
-      <c r="AE28" s="35">
+      <c r="AE28" s="19">
         <f>H28/10</f>
         <v>0.5</v>
       </c>
-      <c r="AF28" s="33">
+      <c r="AF28" s="17">
         <f>J28/10</f>
         <v>0.2</v>
       </c>
-      <c r="AG28" s="32">
+      <c r="AG28" s="16">
         <f>L28/10</f>
         <v>0.5</v>
       </c>
-      <c r="AH28" s="34">
+      <c r="AH28" s="18">
         <f>N28/10</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C29" s="21">
+      <c r="C29" s="9">
         <v>0.2</v>
       </c>
       <c r="D29" s="3">
@@ -2240,46 +2252,46 @@
       <c r="O29" s="2">
         <v>10</v>
       </c>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-      <c r="AB29" s="21">
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="36"/>
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AB29" s="9">
         <v>0.2</v>
       </c>
-      <c r="AC29" s="32">
+      <c r="AC29" s="16">
         <f t="shared" ref="AC29:AC37" si="6">D29/10</f>
         <v>0.7</v>
       </c>
-      <c r="AD29" s="34">
+      <c r="AD29" s="18">
         <f t="shared" ref="AD29:AD37" si="7">F29/10</f>
         <v>0.2</v>
       </c>
-      <c r="AE29" s="35">
+      <c r="AE29" s="19">
         <f t="shared" ref="AE29:AE37" si="8">H29/10</f>
         <v>0.8</v>
       </c>
-      <c r="AF29" s="33">
+      <c r="AF29" s="17">
         <f t="shared" ref="AF29:AF37" si="9">J29/10</f>
         <v>0.2</v>
       </c>
-      <c r="AG29" s="32">
+      <c r="AG29" s="16">
         <f t="shared" ref="AG29:AG37" si="10">L29/10</f>
         <v>0.3</v>
       </c>
-      <c r="AH29" s="34">
+      <c r="AH29" s="18">
         <f t="shared" ref="AH29:AH37" si="11">N29/10</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C30" s="21">
+      <c r="C30" s="9">
         <v>0.3</v>
       </c>
       <c r="D30" s="3">
@@ -2318,46 +2330,46 @@
       <c r="O30" s="2">
         <v>10</v>
       </c>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-      <c r="AB30" s="21">
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AB30" s="9">
         <v>0.3</v>
       </c>
-      <c r="AC30" s="32">
+      <c r="AC30" s="16">
         <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
-      <c r="AD30" s="34">
+      <c r="AD30" s="18">
         <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
-      <c r="AE30" s="35">
+      <c r="AE30" s="19">
         <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
-      <c r="AF30" s="33">
+      <c r="AF30" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG30" s="32">
+      <c r="AG30" s="16">
         <f t="shared" si="10"/>
         <v>0.1</v>
       </c>
-      <c r="AH30" s="34">
+      <c r="AH30" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C31" s="21">
+      <c r="C31" s="9">
         <v>0.4</v>
       </c>
       <c r="D31" s="3">
@@ -2396,46 +2408,46 @@
       <c r="O31" s="2">
         <v>10</v>
       </c>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AB31" s="21">
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AB31" s="9">
         <v>0.4</v>
       </c>
-      <c r="AC31" s="32">
+      <c r="AC31" s="16">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AD31" s="34">
+      <c r="AD31" s="18">
         <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
-      <c r="AE31" s="35">
+      <c r="AE31" s="19">
         <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
-      <c r="AF31" s="33">
+      <c r="AF31" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG31" s="32">
+      <c r="AG31" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH31" s="34">
+      <c r="AH31" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C32" s="21">
+      <c r="C32" s="9">
         <v>0.5</v>
       </c>
       <c r="D32" s="3">
@@ -2474,46 +2486,46 @@
       <c r="O32" s="2">
         <v>10</v>
       </c>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AB32" s="21">
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AB32" s="9">
         <v>0.5</v>
       </c>
-      <c r="AC32" s="32">
+      <c r="AC32" s="16">
         <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
-      <c r="AD32" s="34">
+      <c r="AD32" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE32" s="35">
+      <c r="AE32" s="19">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AF32" s="33">
+      <c r="AF32" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG32" s="32">
+      <c r="AG32" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH32" s="34">
+      <c r="AH32" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C33" s="21">
+      <c r="C33" s="9">
         <v>0.6</v>
       </c>
       <c r="D33" s="3">
@@ -2552,46 +2564,46 @@
       <c r="O33" s="2">
         <v>10</v>
       </c>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-      <c r="AB33" s="21">
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AB33" s="9">
         <v>0.6</v>
       </c>
-      <c r="AC33" s="32">
+      <c r="AC33" s="16">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AD33" s="34">
+      <c r="AD33" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE33" s="35">
+      <c r="AE33" s="19">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="AF33" s="33">
+      <c r="AF33" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="32">
+      <c r="AG33" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH33" s="34">
+      <c r="AH33" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C34" s="21">
+      <c r="C34" s="9">
         <v>0.7</v>
       </c>
       <c r="D34" s="3">
@@ -2630,50 +2642,50 @@
       <c r="O34" s="2">
         <v>10</v>
       </c>
-      <c r="Q34" s="8" t="s">
+      <c r="Q34" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="9" t="s">
+      <c r="R34" s="44"/>
+      <c r="S34" s="44"/>
+      <c r="T34" s="44"/>
+      <c r="U34" s="44"/>
+      <c r="V34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="Y34" s="9"/>
-      <c r="Z34" s="9"/>
-      <c r="AB34" s="21">
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
+      <c r="AB34" s="9">
         <v>0.7</v>
       </c>
-      <c r="AC34" s="32">
+      <c r="AC34" s="16">
         <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
-      <c r="AD34" s="34">
+      <c r="AD34" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE34" s="35">
+      <c r="AE34" s="19">
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="AF34" s="33">
+      <c r="AF34" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="32">
+      <c r="AG34" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH34" s="34">
+      <c r="AH34" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C35" s="21">
+      <c r="C35" s="9">
         <v>0.8</v>
       </c>
       <c r="D35" s="3">
@@ -2712,46 +2724,46 @@
       <c r="O35" s="2">
         <v>10</v>
       </c>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AB35" s="21">
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="36"/>
+      <c r="W35" s="36"/>
+      <c r="X35" s="36"/>
+      <c r="Y35" s="36"/>
+      <c r="Z35" s="36"/>
+      <c r="AB35" s="9">
         <v>0.8</v>
       </c>
-      <c r="AC35" s="32">
+      <c r="AC35" s="16">
         <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
-      <c r="AD35" s="34">
+      <c r="AD35" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE35" s="35">
+      <c r="AE35" s="19">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="AF35" s="33">
+      <c r="AF35" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG35" s="32">
+      <c r="AG35" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH35" s="34">
+      <c r="AH35" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C36" s="21">
+      <c r="C36" s="9">
         <v>0.9</v>
       </c>
       <c r="D36" s="3">
@@ -2790,46 +2802,46 @@
       <c r="O36" s="2">
         <v>10</v>
       </c>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AB36" s="21">
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="36"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="36"/>
+      <c r="Z36" s="36"/>
+      <c r="AB36" s="9">
         <v>0.9</v>
       </c>
-      <c r="AC36" s="32">
+      <c r="AC36" s="16">
         <f t="shared" si="6"/>
         <v>0.7</v>
       </c>
-      <c r="AD36" s="34">
+      <c r="AD36" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE36" s="35">
+      <c r="AE36" s="19">
         <f t="shared" si="8"/>
         <v>0.1</v>
       </c>
-      <c r="AF36" s="33">
+      <c r="AF36" s="17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG36" s="32">
+      <c r="AG36" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH36" s="34">
+      <c r="AH36" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="22">
+      <c r="C37" s="10">
         <v>1</v>
       </c>
       <c r="D37" s="5">
@@ -2868,255 +2880,227 @@
       <c r="O37" s="6">
         <v>10</v>
       </c>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AB37" s="22">
-        <v>1</v>
-      </c>
-      <c r="AC37" s="36">
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="36"/>
+      <c r="W37" s="36"/>
+      <c r="X37" s="36"/>
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="36"/>
+      <c r="AB37" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="20">
         <f t="shared" si="6"/>
         <v>0.7</v>
       </c>
-      <c r="AD37" s="37">
+      <c r="AD37" s="21">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE37" s="38">
+      <c r="AE37" s="22">
         <f t="shared" si="8"/>
         <v>0.1</v>
       </c>
-      <c r="AF37" s="39">
+      <c r="AF37" s="23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AG37" s="36">
+      <c r="AG37" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AH37" s="37">
+      <c r="AH37" s="21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
-      <c r="X38" s="9"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="9"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="36"/>
+      <c r="W38" s="36"/>
+      <c r="X38" s="36"/>
+      <c r="Y38" s="36"/>
+      <c r="Z38" s="36"/>
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="36"/>
+      <c r="X39" s="36"/>
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="36"/>
     </row>
     <row r="40" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q40" s="8" t="s">
+      <c r="Q40" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="9" t="s">
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="W40" s="9"/>
-      <c r="X40" s="9"/>
-      <c r="Y40" s="9"/>
-      <c r="Z40" s="9"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="36"/>
     </row>
     <row r="41" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="9"/>
-      <c r="W41" s="9"/>
-      <c r="X41" s="9"/>
-      <c r="Y41" s="9"/>
-      <c r="Z41" s="9"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="36"/>
+      <c r="W41" s="36"/>
+      <c r="X41" s="36"/>
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="36"/>
     </row>
     <row r="42" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="9"/>
-      <c r="W42" s="9"/>
-      <c r="X42" s="9"/>
-      <c r="Y42" s="9"/>
-      <c r="Z42" s="9"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+      <c r="U42" s="44"/>
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="36"/>
+      <c r="Z42" s="36"/>
     </row>
     <row r="43" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="9"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="36"/>
+      <c r="W43" s="36"/>
+      <c r="X43" s="36"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
     </row>
     <row r="44" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="44"/>
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="36"/>
+      <c r="W44" s="36"/>
+      <c r="X44" s="36"/>
+      <c r="Y44" s="36"/>
+      <c r="Z44" s="36"/>
     </row>
     <row r="45" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="9"/>
-      <c r="Y45" s="9"/>
-      <c r="Z45" s="9"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="44"/>
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
+      <c r="U45" s="44"/>
+      <c r="V45" s="36"/>
+      <c r="W45" s="36"/>
+      <c r="X45" s="36"/>
+      <c r="Y45" s="36"/>
+      <c r="Z45" s="36"/>
     </row>
     <row r="46" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q46" s="9" t="s">
+      <c r="Q46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
+      <c r="R46" s="45"/>
+      <c r="S46" s="45"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="45"/>
     </row>
     <row r="47" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
+      <c r="Q47" s="45"/>
+      <c r="R47" s="45"/>
+      <c r="S47" s="45"/>
+      <c r="T47" s="45"/>
+      <c r="U47" s="45"/>
     </row>
     <row r="48" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="45"/>
+      <c r="S48" s="45"/>
+      <c r="T48" s="45"/>
+      <c r="U48" s="45"/>
     </row>
     <row r="49" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="45"/>
+      <c r="T49" s="45"/>
+      <c r="U49" s="45"/>
     </row>
     <row r="50" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="45"/>
+      <c r="S50" s="45"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="45"/>
     </row>
     <row r="51" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q51" s="9"/>
-      <c r="R51" s="9"/>
-      <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="45"/>
+      <c r="S51" s="45"/>
+      <c r="T51" s="45"/>
+      <c r="U51" s="45"/>
     </row>
     <row r="52" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q52" s="8" t="s">
+      <c r="Q52" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
+      <c r="R52" s="44"/>
+      <c r="S52" s="44"/>
+      <c r="T52" s="44"/>
+      <c r="U52" s="44"/>
     </row>
     <row r="53" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="8"/>
-      <c r="U53" s="8"/>
+      <c r="Q53" s="44"/>
+      <c r="R53" s="44"/>
+      <c r="S53" s="44"/>
+      <c r="T53" s="44"/>
+      <c r="U53" s="44"/>
     </row>
     <row r="54" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q54" s="8"/>
-      <c r="R54" s="8"/>
-      <c r="S54" s="8"/>
-      <c r="T54" s="8"/>
-      <c r="U54" s="8"/>
+      <c r="Q54" s="44"/>
+      <c r="R54" s="44"/>
+      <c r="S54" s="44"/>
+      <c r="T54" s="44"/>
+      <c r="U54" s="44"/>
     </row>
     <row r="55" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
-      <c r="S55" s="8"/>
-      <c r="T55" s="8"/>
-      <c r="U55" s="8"/>
+      <c r="Q55" s="44"/>
+      <c r="R55" s="44"/>
+      <c r="S55" s="44"/>
+      <c r="T55" s="44"/>
+      <c r="U55" s="44"/>
     </row>
     <row r="56" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="T56" s="8"/>
-      <c r="U56" s="8"/>
+      <c r="Q56" s="44"/>
+      <c r="R56" s="44"/>
+      <c r="S56" s="44"/>
+      <c r="T56" s="44"/>
+      <c r="U56" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="AB9:AH9"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AB25:AH25"/>
-    <mergeCell ref="V11:Z13"/>
-    <mergeCell ref="V14:Z16"/>
-    <mergeCell ref="V17:Z19"/>
-    <mergeCell ref="Q20:U22"/>
-    <mergeCell ref="V20:Z22"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="C9:O9"/>
-    <mergeCell ref="C25:O25"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="Q11:U13"/>
-    <mergeCell ref="Q14:U16"/>
-    <mergeCell ref="Q17:U19"/>
     <mergeCell ref="Q52:U56"/>
     <mergeCell ref="V28:Z33"/>
     <mergeCell ref="V34:Z39"/>
@@ -3125,6 +3109,34 @@
     <mergeCell ref="Q34:U39"/>
     <mergeCell ref="Q40:U45"/>
     <mergeCell ref="Q46:U51"/>
+    <mergeCell ref="C9:O9"/>
+    <mergeCell ref="C25:O25"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="Q11:U13"/>
+    <mergeCell ref="Q14:U16"/>
+    <mergeCell ref="Q17:U19"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="V11:Z13"/>
+    <mergeCell ref="V14:Z16"/>
+    <mergeCell ref="V17:Z19"/>
+    <mergeCell ref="Q20:U22"/>
+    <mergeCell ref="V20:Z22"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AB25:AH25"/>
+    <mergeCell ref="AB9:AH9"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed tests for parameters, updated accordingly chap 4.2, added notes on integration with Insight
</commit_message>
<xml_diff>
--- a/praca/badania/badanie2.xlsx
+++ b/praca/badania/badanie2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abani\Desktop\Praca magisterska\praca\badania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD5A54C-9810-48DE-8068-DDAB08DC7D74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0885E671-B7EA-4D05-9E3B-73292414C341}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="23">
   <si>
     <t>NS+</t>
   </si>
@@ -639,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,13 +670,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -688,13 +697,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -706,24 +715,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1004,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:AH56"/>
+  <dimension ref="C4:AH89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28:U33"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V70" sqref="V70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,21 +1033,21 @@
     </row>
     <row r="8" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="42"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="33"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
         <v>1</v>
@@ -1054,38 +1061,38 @@
       <c r="U9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB9" s="28" t="s">
+      <c r="AB9" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="AC9" s="29"/>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="29"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="30"/>
+      <c r="AC9" s="44"/>
+      <c r="AD9" s="44"/>
+      <c r="AE9" s="44"/>
+      <c r="AF9" s="44"/>
+      <c r="AG9" s="44"/>
+      <c r="AH9" s="45"/>
     </row>
     <row r="10" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="37" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="37" t="s">
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="39"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
       <c r="Q10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1101,24 +1108,24 @@
       <c r="U10" s="2">
         <v>5</v>
       </c>
-      <c r="AB10" s="31" t="s">
+      <c r="AB10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AC10" s="33" t="s">
+      <c r="AC10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="34"/>
-      <c r="AE10" s="35" t="s">
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF10" s="34"/>
-      <c r="AG10" s="33" t="s">
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="34"/>
+      <c r="AH10" s="38"/>
     </row>
     <row r="11" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="32"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="5" t="s">
         <v>1</v>
       </c>
@@ -1155,19 +1162,19 @@
       <c r="O11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="43" t="s">
+      <c r="Q11" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="36"/>
-      <c r="Z11" s="36"/>
-      <c r="AB11" s="32"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="46"/>
+      <c r="W11" s="46"/>
+      <c r="X11" s="46"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="46"/>
+      <c r="AB11" s="35"/>
       <c r="AC11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1227,16 +1234,16 @@
       <c r="O12" s="14">
         <v>0</v>
       </c>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="46"/>
       <c r="AB12" s="11">
         <v>0.1</v>
       </c>
@@ -1305,16 +1312,16 @@
       <c r="O13" s="4">
         <v>4</v>
       </c>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="36"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="46"/>
+      <c r="W13" s="46"/>
+      <c r="X13" s="46"/>
+      <c r="Y13" s="46"/>
+      <c r="Z13" s="46"/>
       <c r="AB13" s="9">
         <v>0.2</v>
       </c>
@@ -1383,16 +1390,16 @@
       <c r="O14" s="4">
         <v>4</v>
       </c>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="46"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="46"/>
+      <c r="V14" s="46"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="46"/>
+      <c r="Y14" s="46"/>
+      <c r="Z14" s="46"/>
       <c r="AB14" s="9">
         <v>0.3</v>
       </c>
@@ -1461,16 +1468,16 @@
       <c r="O15" s="4">
         <v>6</v>
       </c>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="36"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
       <c r="AB15" s="9">
         <v>0.4</v>
       </c>
@@ -1539,16 +1546,16 @@
       <c r="O16" s="4">
         <v>10</v>
       </c>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="46"/>
       <c r="AB16" s="9">
         <v>0.5</v>
       </c>
@@ -1617,16 +1624,16 @@
       <c r="O17" s="4">
         <v>10</v>
       </c>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="46"/>
+      <c r="Z17" s="46"/>
       <c r="AB17" s="9">
         <v>0.6</v>
       </c>
@@ -1695,16 +1702,16 @@
       <c r="O18" s="4">
         <v>10</v>
       </c>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="46"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="46"/>
+      <c r="Z18" s="46"/>
       <c r="AB18" s="9">
         <v>0.7</v>
       </c>
@@ -1773,16 +1780,16 @@
       <c r="O19" s="4">
         <v>10</v>
       </c>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="36"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="46"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="46"/>
+      <c r="Y19" s="46"/>
+      <c r="Z19" s="46"/>
       <c r="AB19" s="9">
         <v>0.8</v>
       </c>
@@ -1851,16 +1858,16 @@
       <c r="O20" s="4">
         <v>10</v>
       </c>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="46"/>
+      <c r="Z20" s="46"/>
       <c r="AB20" s="9">
         <v>0.9</v>
       </c>
@@ -1929,16 +1936,16 @@
       <c r="O21" s="7">
         <v>10</v>
       </c>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
+      <c r="U21" s="46"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="46"/>
+      <c r="Y21" s="46"/>
+      <c r="Z21" s="46"/>
       <c r="AB21" s="10">
         <v>1</v>
       </c>
@@ -1968,34 +1975,34 @@
       </c>
     </row>
     <row r="22" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="46"/>
+      <c r="Z22" s="46"/>
     </row>
     <row r="24" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="42"/>
+      <c r="C25" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="33"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2" t="s">
         <v>1</v>
@@ -2009,38 +2016,38 @@
       <c r="U25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB25" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC25" s="29"/>
-      <c r="AD25" s="29"/>
-      <c r="AE25" s="29"/>
-      <c r="AF25" s="29"/>
-      <c r="AG25" s="29"/>
-      <c r="AH25" s="30"/>
+      <c r="AB25" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC25" s="44"/>
+      <c r="AD25" s="44"/>
+      <c r="AE25" s="44"/>
+      <c r="AF25" s="44"/>
+      <c r="AG25" s="44"/>
+      <c r="AH25" s="45"/>
     </row>
     <row r="26" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="37" t="s">
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="37" t="s">
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="39"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="42"/>
       <c r="Q26" s="2" t="s">
         <v>4</v>
       </c>
@@ -2056,24 +2063,24 @@
       <c r="U26" s="2">
         <v>5</v>
       </c>
-      <c r="AB26" s="31" t="s">
+      <c r="AB26" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AC26" s="33" t="s">
+      <c r="AC26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AD26" s="34"/>
-      <c r="AE26" s="35" t="s">
+      <c r="AD26" s="38"/>
+      <c r="AE26" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF26" s="34"/>
-      <c r="AG26" s="33" t="s">
+      <c r="AF26" s="38"/>
+      <c r="AG26" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="AH26" s="34"/>
+      <c r="AH26" s="38"/>
     </row>
     <row r="27" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="32"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="5" t="s">
         <v>1</v>
       </c>
@@ -2110,7 +2117,7 @@
       <c r="O27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AB27" s="32"/>
+      <c r="AB27" s="35"/>
       <c r="AC27" s="5" t="s">
         <v>19</v>
       </c>
@@ -2170,20 +2177,20 @@
       <c r="O28" s="13">
         <v>10</v>
       </c>
-      <c r="Q28" s="36" t="s">
+      <c r="Q28" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36" t="s">
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="36"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
       <c r="AB28" s="11">
         <v>0.1</v>
       </c>
@@ -2252,16 +2259,16 @@
       <c r="O29" s="2">
         <v>10</v>
       </c>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
-      <c r="X29" s="36"/>
-      <c r="Y29" s="36"/>
-      <c r="Z29" s="36"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
       <c r="AB29" s="9">
         <v>0.2</v>
       </c>
@@ -2330,16 +2337,16 @@
       <c r="O30" s="2">
         <v>10</v>
       </c>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="36"/>
-      <c r="U30" s="36"/>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="36"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
       <c r="AB30" s="9">
         <v>0.3</v>
       </c>
@@ -2408,16 +2415,16 @@
       <c r="O31" s="2">
         <v>10</v>
       </c>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="36"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+      <c r="T31" s="29"/>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="29"/>
       <c r="AB31" s="9">
         <v>0.4</v>
       </c>
@@ -2486,16 +2493,16 @@
       <c r="O32" s="2">
         <v>10</v>
       </c>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
       <c r="AB32" s="9">
         <v>0.5</v>
       </c>
@@ -2564,16 +2571,16 @@
       <c r="O33" s="2">
         <v>10</v>
       </c>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="36"/>
-      <c r="U33" s="36"/>
-      <c r="V33" s="36"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="36"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="36"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="29"/>
       <c r="AB33" s="9">
         <v>0.6</v>
       </c>
@@ -2642,20 +2649,20 @@
       <c r="O34" s="2">
         <v>10</v>
       </c>
-      <c r="Q34" s="44" t="s">
+      <c r="Q34" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="R34" s="44"/>
-      <c r="S34" s="44"/>
-      <c r="T34" s="44"/>
-      <c r="U34" s="44"/>
-      <c r="V34" s="36" t="s">
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="W34" s="36"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="36"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
       <c r="AB34" s="9">
         <v>0.7</v>
       </c>
@@ -2724,16 +2731,16 @@
       <c r="O35" s="2">
         <v>10</v>
       </c>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="44"/>
-      <c r="T35" s="44"/>
-      <c r="U35" s="44"/>
-      <c r="V35" s="36"/>
-      <c r="W35" s="36"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="36"/>
-      <c r="Z35" s="36"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="29"/>
       <c r="AB35" s="9">
         <v>0.8</v>
       </c>
@@ -2802,16 +2809,16 @@
       <c r="O36" s="2">
         <v>10</v>
       </c>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="44"/>
-      <c r="S36" s="44"/>
-      <c r="T36" s="44"/>
-      <c r="U36" s="44"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="36"/>
-      <c r="Z36" s="36"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
       <c r="AB36" s="9">
         <v>0.9</v>
       </c>
@@ -2880,16 +2887,16 @@
       <c r="O37" s="6">
         <v>10</v>
       </c>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
-      <c r="T37" s="44"/>
-      <c r="U37" s="44"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="36"/>
+      <c r="Q37" s="28"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="28"/>
+      <c r="T37" s="28"/>
+      <c r="U37" s="28"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
       <c r="AB37" s="10">
         <v>1</v>
       </c>
@@ -2919,188 +2926,1955 @@
       </c>
     </row>
     <row r="38" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q38" s="44"/>
-      <c r="R38" s="44"/>
-      <c r="S38" s="44"/>
-      <c r="T38" s="44"/>
-      <c r="U38" s="44"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="36"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q39" s="44"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="44"/>
-      <c r="T39" s="44"/>
-      <c r="U39" s="44"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
     </row>
     <row r="40" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q40" s="44" t="s">
+      <c r="Q40" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R40" s="44"/>
-      <c r="S40" s="44"/>
-      <c r="T40" s="44"/>
-      <c r="U40" s="44"/>
-      <c r="V40" s="36" t="s">
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="36"/>
-      <c r="Z40" s="36"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
     </row>
     <row r="41" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q41" s="44"/>
-      <c r="R41" s="44"/>
-      <c r="S41" s="44"/>
-      <c r="T41" s="44"/>
-      <c r="U41" s="44"/>
-      <c r="V41" s="36"/>
-      <c r="W41" s="36"/>
-      <c r="X41" s="36"/>
-      <c r="Y41" s="36"/>
-      <c r="Z41" s="36"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="28"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
     </row>
     <row r="42" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q42" s="44"/>
-      <c r="R42" s="44"/>
-      <c r="S42" s="44"/>
-      <c r="T42" s="44"/>
-      <c r="U42" s="44"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="36"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
     </row>
     <row r="43" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="44"/>
-      <c r="V43" s="36"/>
-      <c r="W43" s="36"/>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="36"/>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="28"/>
+      <c r="U43" s="28"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
     </row>
     <row r="44" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="44"/>
-      <c r="U44" s="44"/>
-      <c r="V44" s="36"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="36"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="28"/>
+      <c r="U44" s="28"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
     </row>
     <row r="45" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
-      <c r="V45" s="36"/>
-      <c r="W45" s="36"/>
-      <c r="X45" s="36"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="36"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="28"/>
+      <c r="U45" s="28"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="29"/>
+      <c r="X45" s="29"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="29"/>
     </row>
     <row r="46" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q46" s="45" t="s">
+      <c r="Q46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="R46" s="45"/>
-      <c r="S46" s="45"/>
-      <c r="T46" s="45"/>
-      <c r="U46" s="45"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
     </row>
     <row r="47" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="45"/>
-      <c r="U47" s="45"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
     </row>
     <row r="48" spans="3:34" x14ac:dyDescent="0.25">
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="45"/>
-      <c r="U48" s="45"/>
-    </row>
-    <row r="49" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q49" s="45"/>
-      <c r="R49" s="45"/>
-      <c r="S49" s="45"/>
-      <c r="T49" s="45"/>
-      <c r="U49" s="45"/>
-    </row>
-    <row r="50" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q50" s="45"/>
-      <c r="R50" s="45"/>
-      <c r="S50" s="45"/>
-      <c r="T50" s="45"/>
-      <c r="U50" s="45"/>
-    </row>
-    <row r="51" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q51" s="45"/>
-      <c r="R51" s="45"/>
-      <c r="S51" s="45"/>
-      <c r="T51" s="45"/>
-      <c r="U51" s="45"/>
-    </row>
-    <row r="52" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q52" s="44" t="s">
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+    </row>
+    <row r="49" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q49" s="30"/>
+      <c r="R49" s="30"/>
+      <c r="S49" s="30"/>
+      <c r="T49" s="30"/>
+      <c r="U49" s="30"/>
+    </row>
+    <row r="50" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q50" s="30"/>
+      <c r="R50" s="30"/>
+      <c r="S50" s="30"/>
+      <c r="T50" s="30"/>
+      <c r="U50" s="30"/>
+    </row>
+    <row r="51" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="30"/>
+      <c r="T51" s="30"/>
+      <c r="U51" s="30"/>
+    </row>
+    <row r="52" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q52" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="R52" s="44"/>
-      <c r="S52" s="44"/>
-      <c r="T52" s="44"/>
-      <c r="U52" s="44"/>
-    </row>
-    <row r="53" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q53" s="44"/>
-      <c r="R53" s="44"/>
-      <c r="S53" s="44"/>
-      <c r="T53" s="44"/>
-      <c r="U53" s="44"/>
-    </row>
-    <row r="54" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q54" s="44"/>
-      <c r="R54" s="44"/>
-      <c r="S54" s="44"/>
-      <c r="T54" s="44"/>
-      <c r="U54" s="44"/>
-    </row>
-    <row r="55" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q55" s="44"/>
-      <c r="R55" s="44"/>
-      <c r="S55" s="44"/>
-      <c r="T55" s="44"/>
-      <c r="U55" s="44"/>
-    </row>
-    <row r="56" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q56" s="44"/>
-      <c r="R56" s="44"/>
-      <c r="S56" s="44"/>
-      <c r="T56" s="44"/>
-      <c r="U56" s="44"/>
+      <c r="R52" s="28"/>
+      <c r="S52" s="28"/>
+      <c r="T52" s="28"/>
+      <c r="U52" s="28"/>
+    </row>
+    <row r="53" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q53" s="28"/>
+      <c r="R53" s="28"/>
+      <c r="S53" s="28"/>
+      <c r="T53" s="28"/>
+      <c r="U53" s="28"/>
+    </row>
+    <row r="54" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q54" s="28"/>
+      <c r="R54" s="28"/>
+      <c r="S54" s="28"/>
+      <c r="T54" s="28"/>
+      <c r="U54" s="28"/>
+    </row>
+    <row r="55" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q55" s="28"/>
+      <c r="R55" s="28"/>
+      <c r="S55" s="28"/>
+      <c r="T55" s="28"/>
+      <c r="U55" s="28"/>
+    </row>
+    <row r="56" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="Q56" s="28"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="28"/>
+      <c r="T56" s="28"/>
+      <c r="U56" s="28"/>
+    </row>
+    <row r="58" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="44"/>
+      <c r="M59" s="44"/>
+      <c r="N59" s="44"/>
+      <c r="O59" s="45"/>
+      <c r="Q59" s="48"/>
+      <c r="R59" s="48"/>
+      <c r="S59" s="48"/>
+      <c r="T59" s="48"/>
+      <c r="U59" s="48"/>
+      <c r="AB59" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC59" s="44"/>
+      <c r="AD59" s="44"/>
+      <c r="AE59" s="44"/>
+      <c r="AF59" s="44"/>
+      <c r="AG59" s="44"/>
+      <c r="AH59" s="45"/>
+    </row>
+    <row r="60" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C60" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="38"/>
+      <c r="Q60" s="48"/>
+      <c r="R60" s="48"/>
+      <c r="S60" s="48"/>
+      <c r="T60" s="48"/>
+      <c r="U60" s="48"/>
+      <c r="AB60" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC60" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD60" s="38"/>
+      <c r="AE60" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF60" s="38"/>
+      <c r="AG60" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH60" s="38"/>
+    </row>
+    <row r="61" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="35"/>
+      <c r="D61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O61" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="47"/>
+      <c r="R61" s="47"/>
+      <c r="S61" s="47"/>
+      <c r="T61" s="47"/>
+      <c r="U61" s="47"/>
+      <c r="V61" s="46"/>
+      <c r="W61" s="46"/>
+      <c r="X61" s="46"/>
+      <c r="Y61" s="46"/>
+      <c r="Z61" s="46"/>
+      <c r="AB61" s="35"/>
+      <c r="AC61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF61" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH61" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C62" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D62" s="12">
+        <v>0</v>
+      </c>
+      <c r="E62" s="13">
+        <v>10</v>
+      </c>
+      <c r="F62" s="13">
+        <v>10</v>
+      </c>
+      <c r="G62" s="14">
+        <v>0</v>
+      </c>
+      <c r="H62" s="12">
+        <v>0</v>
+      </c>
+      <c r="I62" s="13">
+        <v>10</v>
+      </c>
+      <c r="J62" s="13">
+        <v>10</v>
+      </c>
+      <c r="K62" s="14">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
+        <v>0</v>
+      </c>
+      <c r="M62" s="13">
+        <v>10</v>
+      </c>
+      <c r="N62" s="13">
+        <v>10</v>
+      </c>
+      <c r="O62" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="47"/>
+      <c r="R62" s="47"/>
+      <c r="S62" s="47"/>
+      <c r="T62" s="47"/>
+      <c r="U62" s="47"/>
+      <c r="V62" s="46"/>
+      <c r="W62" s="46"/>
+      <c r="X62" s="46"/>
+      <c r="Y62" s="46"/>
+      <c r="Z62" s="46"/>
+      <c r="AB62" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="AC62" s="16">
+        <f>D62/10</f>
+        <v>0</v>
+      </c>
+      <c r="AD62" s="18">
+        <f>F62/10</f>
+        <v>1</v>
+      </c>
+      <c r="AE62" s="19">
+        <f>H62/10</f>
+        <v>0</v>
+      </c>
+      <c r="AF62" s="17">
+        <f>J62/10</f>
+        <v>1</v>
+      </c>
+      <c r="AG62" s="16">
+        <f>L62/10</f>
+        <v>0</v>
+      </c>
+      <c r="AH62" s="18">
+        <f>N62/10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C63" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>10</v>
+      </c>
+      <c r="F63" s="2">
+        <v>10</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>10</v>
+      </c>
+      <c r="J63" s="2">
+        <v>10</v>
+      </c>
+      <c r="K63" s="4">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3">
+        <v>3</v>
+      </c>
+      <c r="M63" s="2">
+        <v>7</v>
+      </c>
+      <c r="N63" s="2">
+        <v>6</v>
+      </c>
+      <c r="O63" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q63" s="47"/>
+      <c r="R63" s="47"/>
+      <c r="S63" s="47"/>
+      <c r="T63" s="47"/>
+      <c r="U63" s="47"/>
+      <c r="V63" s="46"/>
+      <c r="W63" s="46"/>
+      <c r="X63" s="46"/>
+      <c r="Y63" s="46"/>
+      <c r="Z63" s="46"/>
+      <c r="AB63" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="AC63" s="16">
+        <f>D63/10</f>
+        <v>0</v>
+      </c>
+      <c r="AD63" s="18">
+        <f>F63/10</f>
+        <v>1</v>
+      </c>
+      <c r="AE63" s="19">
+        <f>H63/10</f>
+        <v>0</v>
+      </c>
+      <c r="AF63" s="17">
+        <f>J63/10</f>
+        <v>1</v>
+      </c>
+      <c r="AG63" s="16">
+        <f>L63/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="AH63" s="18">
+        <f>N63/10</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="64" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C64" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>10</v>
+      </c>
+      <c r="F64" s="2">
+        <v>10</v>
+      </c>
+      <c r="G64" s="4">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>2</v>
+      </c>
+      <c r="I64" s="2">
+        <v>8</v>
+      </c>
+      <c r="J64" s="2">
+        <v>7</v>
+      </c>
+      <c r="K64" s="4">
+        <v>3</v>
+      </c>
+      <c r="L64" s="3">
+        <v>4</v>
+      </c>
+      <c r="M64" s="2">
+        <v>6</v>
+      </c>
+      <c r="N64" s="2">
+        <v>6</v>
+      </c>
+      <c r="O64" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q64" s="46"/>
+      <c r="R64" s="46"/>
+      <c r="S64" s="46"/>
+      <c r="T64" s="46"/>
+      <c r="U64" s="46"/>
+      <c r="V64" s="46"/>
+      <c r="W64" s="46"/>
+      <c r="X64" s="46"/>
+      <c r="Y64" s="46"/>
+      <c r="Z64" s="46"/>
+      <c r="AB64" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="AC64" s="16">
+        <f>D64/10</f>
+        <v>0</v>
+      </c>
+      <c r="AD64" s="18">
+        <f>F64/10</f>
+        <v>1</v>
+      </c>
+      <c r="AE64" s="19">
+        <f>H64/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AF64" s="17">
+        <f>J64/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="AG64" s="16">
+        <f>L64/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="AH64" s="18">
+        <f>N64/10</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="65" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C65" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2">
+        <v>9</v>
+      </c>
+      <c r="F65" s="2">
+        <v>9</v>
+      </c>
+      <c r="G65" s="4">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3">
+        <v>4</v>
+      </c>
+      <c r="I65" s="2">
+        <v>6</v>
+      </c>
+      <c r="J65" s="2">
+        <v>5</v>
+      </c>
+      <c r="K65" s="4">
+        <v>5</v>
+      </c>
+      <c r="L65" s="3">
+        <v>4</v>
+      </c>
+      <c r="M65" s="2">
+        <v>6</v>
+      </c>
+      <c r="N65" s="2">
+        <v>4</v>
+      </c>
+      <c r="O65" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q65" s="46"/>
+      <c r="R65" s="46"/>
+      <c r="S65" s="46"/>
+      <c r="T65" s="46"/>
+      <c r="U65" s="46"/>
+      <c r="V65" s="46"/>
+      <c r="W65" s="46"/>
+      <c r="X65" s="46"/>
+      <c r="Y65" s="46"/>
+      <c r="Z65" s="46"/>
+      <c r="AB65" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="AC65" s="16">
+        <f t="shared" ref="AC65:AC71" si="12">D65/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="AD65" s="18">
+        <f t="shared" ref="AD65:AD71" si="13">F65/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE65" s="19">
+        <f t="shared" ref="AE65:AE71" si="14">H65/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="AF65" s="17">
+        <f t="shared" ref="AF65:AF71" si="15">J65/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="AG65" s="16">
+        <f t="shared" ref="AG65:AG71" si="16">L65/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="AH65" s="18">
+        <f t="shared" ref="AH65:AH71" si="17">N65/10</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="66" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C66" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D66" s="3">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2">
+        <v>9</v>
+      </c>
+      <c r="F66" s="2">
+        <v>9</v>
+      </c>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+      <c r="H66" s="3">
+        <v>1</v>
+      </c>
+      <c r="I66" s="27">
+        <v>9</v>
+      </c>
+      <c r="J66" s="27">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <v>10</v>
+      </c>
+      <c r="L66" s="3">
+        <v>1</v>
+      </c>
+      <c r="M66" s="2">
+        <v>9</v>
+      </c>
+      <c r="N66" s="2">
+        <v>0</v>
+      </c>
+      <c r="O66" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="46"/>
+      <c r="S66" s="46"/>
+      <c r="T66" s="46"/>
+      <c r="U66" s="46"/>
+      <c r="V66" s="46"/>
+      <c r="W66" s="46"/>
+      <c r="X66" s="46"/>
+      <c r="Y66" s="46"/>
+      <c r="Z66" s="46"/>
+      <c r="AB66" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="AC66" s="16">
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="AD66" s="18">
+        <f t="shared" si="13"/>
+        <v>0.9</v>
+      </c>
+      <c r="AE66" s="19">
+        <f t="shared" si="14"/>
+        <v>0.1</v>
+      </c>
+      <c r="AF66" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG66" s="16">
+        <f t="shared" si="16"/>
+        <v>0.1</v>
+      </c>
+      <c r="AH66" s="18">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C67" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="D67" s="3">
+        <v>2</v>
+      </c>
+      <c r="E67" s="2">
+        <v>8</v>
+      </c>
+      <c r="F67" s="2">
+        <v>7</v>
+      </c>
+      <c r="G67" s="4">
+        <v>3</v>
+      </c>
+      <c r="H67" s="8">
+        <v>0</v>
+      </c>
+      <c r="I67" s="2">
+        <v>10</v>
+      </c>
+      <c r="J67" s="2">
+        <v>0</v>
+      </c>
+      <c r="K67" s="25">
+        <v>10</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0</v>
+      </c>
+      <c r="M67" s="2">
+        <v>10</v>
+      </c>
+      <c r="N67" s="2">
+        <v>0</v>
+      </c>
+      <c r="O67" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q67" s="46"/>
+      <c r="R67" s="46"/>
+      <c r="S67" s="46"/>
+      <c r="T67" s="46"/>
+      <c r="U67" s="46"/>
+      <c r="V67" s="46"/>
+      <c r="W67" s="46"/>
+      <c r="X67" s="46"/>
+      <c r="Y67" s="46"/>
+      <c r="Z67" s="46"/>
+      <c r="AB67" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="AC67" s="16">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="AD67" s="18">
+        <f t="shared" si="13"/>
+        <v>0.7</v>
+      </c>
+      <c r="AE67" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AF67" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG67" s="16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AH67" s="18">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C68" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="2">
+        <v>8</v>
+      </c>
+      <c r="F68" s="2">
+        <v>6</v>
+      </c>
+      <c r="G68" s="4">
+        <v>4</v>
+      </c>
+      <c r="H68" s="8">
+        <v>0</v>
+      </c>
+      <c r="I68" s="2">
+        <v>10</v>
+      </c>
+      <c r="J68" s="2">
+        <v>0</v>
+      </c>
+      <c r="K68" s="25">
+        <v>10</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+      <c r="M68" s="2">
+        <v>10</v>
+      </c>
+      <c r="N68" s="2">
+        <v>0</v>
+      </c>
+      <c r="O68" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q68" s="46"/>
+      <c r="R68" s="46"/>
+      <c r="S68" s="46"/>
+      <c r="T68" s="46"/>
+      <c r="U68" s="46"/>
+      <c r="V68" s="46"/>
+      <c r="W68" s="46"/>
+      <c r="X68" s="46"/>
+      <c r="Y68" s="46"/>
+      <c r="Z68" s="46"/>
+      <c r="AB68" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="AC68" s="16">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="AD68" s="18">
+        <f t="shared" si="13"/>
+        <v>0.6</v>
+      </c>
+      <c r="AE68" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AF68" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG68" s="16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AH68" s="18">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C69" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D69" s="3">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2">
+        <v>9</v>
+      </c>
+      <c r="F69" s="2">
+        <v>2</v>
+      </c>
+      <c r="G69" s="4">
+        <v>8</v>
+      </c>
+      <c r="H69" s="8">
+        <v>0</v>
+      </c>
+      <c r="I69" s="2">
+        <v>10</v>
+      </c>
+      <c r="J69" s="2">
+        <v>0</v>
+      </c>
+      <c r="K69" s="25">
+        <v>10</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0</v>
+      </c>
+      <c r="M69" s="2">
+        <v>10</v>
+      </c>
+      <c r="N69" s="2">
+        <v>0</v>
+      </c>
+      <c r="O69" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q69" s="46"/>
+      <c r="R69" s="46"/>
+      <c r="S69" s="46"/>
+      <c r="T69" s="46"/>
+      <c r="U69" s="46"/>
+      <c r="V69" s="46"/>
+      <c r="W69" s="46"/>
+      <c r="X69" s="46"/>
+      <c r="Y69" s="46"/>
+      <c r="Z69" s="46"/>
+      <c r="AB69" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="AC69" s="16">
+        <f t="shared" si="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="AD69" s="18">
+        <f t="shared" si="13"/>
+        <v>0.2</v>
+      </c>
+      <c r="AE69" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AF69" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG69" s="16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AH69" s="18">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C70" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>10</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0</v>
+      </c>
+      <c r="G70" s="4">
+        <v>10</v>
+      </c>
+      <c r="H70" s="8">
+        <v>0</v>
+      </c>
+      <c r="I70" s="2">
+        <v>10</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0</v>
+      </c>
+      <c r="K70" s="25">
+        <v>10</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+      <c r="M70" s="2">
+        <v>10</v>
+      </c>
+      <c r="N70" s="2">
+        <v>0</v>
+      </c>
+      <c r="O70" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q70" s="46"/>
+      <c r="R70" s="46"/>
+      <c r="S70" s="46"/>
+      <c r="T70" s="46"/>
+      <c r="U70" s="46"/>
+      <c r="V70" s="46"/>
+      <c r="W70" s="46"/>
+      <c r="X70" s="46"/>
+      <c r="Y70" s="46"/>
+      <c r="Z70" s="46"/>
+      <c r="AB70" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="AC70" s="16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AD70" s="18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AE70" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AF70" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG70" s="16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AH70" s="18">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="10">
+        <v>1</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0</v>
+      </c>
+      <c r="E71" s="6">
+        <v>10</v>
+      </c>
+      <c r="F71" s="6">
+        <v>0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>10</v>
+      </c>
+      <c r="H71" s="24">
+        <v>0</v>
+      </c>
+      <c r="I71" s="6">
+        <v>10</v>
+      </c>
+      <c r="J71" s="6">
+        <v>0</v>
+      </c>
+      <c r="K71" s="26">
+        <v>10</v>
+      </c>
+      <c r="L71" s="5">
+        <v>0</v>
+      </c>
+      <c r="M71" s="6">
+        <v>10</v>
+      </c>
+      <c r="N71" s="6">
+        <v>0</v>
+      </c>
+      <c r="O71" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q71" s="46"/>
+      <c r="R71" s="46"/>
+      <c r="S71" s="46"/>
+      <c r="T71" s="46"/>
+      <c r="U71" s="46"/>
+      <c r="V71" s="46"/>
+      <c r="W71" s="46"/>
+      <c r="X71" s="46"/>
+      <c r="Y71" s="46"/>
+      <c r="Z71" s="46"/>
+      <c r="AB71" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC71" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AD71" s="21">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AE71" s="22">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AF71" s="23">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG71" s="20">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AH71" s="21">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="32"/>
+      <c r="K77" s="32"/>
+      <c r="L77" s="32"/>
+      <c r="M77" s="32"/>
+      <c r="N77" s="32"/>
+      <c r="O77" s="33"/>
+      <c r="AB77" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC77" s="44"/>
+      <c r="AD77" s="44"/>
+      <c r="AE77" s="44"/>
+      <c r="AF77" s="44"/>
+      <c r="AG77" s="44"/>
+      <c r="AH77" s="45"/>
+    </row>
+    <row r="78" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C78" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I78" s="41"/>
+      <c r="J78" s="41"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="M78" s="41"/>
+      <c r="N78" s="41"/>
+      <c r="O78" s="42"/>
+      <c r="AB78" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC78" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD78" s="38"/>
+      <c r="AE78" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF78" s="38"/>
+      <c r="AG78" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH78" s="38"/>
+    </row>
+    <row r="79" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="35"/>
+      <c r="D79" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L79" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N79" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O79" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB79" s="35"/>
+      <c r="AC79" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE79" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF79" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG79" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH79" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C80" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D80" s="12">
+        <v>4</v>
+      </c>
+      <c r="E80" s="13">
+        <v>6</v>
+      </c>
+      <c r="F80" s="13">
+        <v>3</v>
+      </c>
+      <c r="G80" s="13">
+        <v>7</v>
+      </c>
+      <c r="H80" s="12">
+        <v>10</v>
+      </c>
+      <c r="I80" s="13">
+        <v>0</v>
+      </c>
+      <c r="J80" s="13">
+        <v>2</v>
+      </c>
+      <c r="K80" s="13">
+        <v>8</v>
+      </c>
+      <c r="L80" s="12">
+        <v>9</v>
+      </c>
+      <c r="M80" s="13">
+        <v>1</v>
+      </c>
+      <c r="N80" s="13">
+        <v>0</v>
+      </c>
+      <c r="O80" s="14">
+        <v>10</v>
+      </c>
+      <c r="AB80" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="AC80" s="16">
+        <f>D80/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="AD80" s="18">
+        <f>F80/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="AE80" s="19">
+        <f>H80/10</f>
+        <v>1</v>
+      </c>
+      <c r="AF80" s="17">
+        <f>J80/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AG80" s="16">
+        <f>L80/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AH80" s="18">
+        <f>N80/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C81" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D81" s="3">
+        <v>5</v>
+      </c>
+      <c r="E81" s="2">
+        <v>5</v>
+      </c>
+      <c r="F81" s="2">
+        <v>2</v>
+      </c>
+      <c r="G81" s="2">
+        <v>8</v>
+      </c>
+      <c r="H81" s="3">
+        <v>10</v>
+      </c>
+      <c r="I81" s="2">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2">
+        <v>2</v>
+      </c>
+      <c r="K81" s="2">
+        <v>8</v>
+      </c>
+      <c r="L81" s="3">
+        <v>6</v>
+      </c>
+      <c r="M81" s="2">
+        <v>4</v>
+      </c>
+      <c r="N81" s="2">
+        <v>0</v>
+      </c>
+      <c r="O81" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB81" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="AC81" s="16">
+        <f t="shared" ref="AC81:AC89" si="18">D81/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="AD81" s="18">
+        <f t="shared" ref="AD81:AD89" si="19">F81/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AE81" s="19">
+        <f t="shared" ref="AE81:AE89" si="20">H81/10</f>
+        <v>1</v>
+      </c>
+      <c r="AF81" s="17">
+        <f t="shared" ref="AF81:AF89" si="21">J81/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AG81" s="16">
+        <f t="shared" ref="AG81:AG89" si="22">L81/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="AH81" s="18">
+        <f t="shared" ref="AH81:AH89" si="23">N81/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C82" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="D82" s="3">
+        <v>7</v>
+      </c>
+      <c r="E82" s="2">
+        <v>3</v>
+      </c>
+      <c r="F82" s="2">
+        <v>2</v>
+      </c>
+      <c r="G82" s="2">
+        <v>8</v>
+      </c>
+      <c r="H82" s="3">
+        <v>10</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2">
+        <v>10</v>
+      </c>
+      <c r="L82" s="3">
+        <v>6</v>
+      </c>
+      <c r="M82" s="2">
+        <v>4</v>
+      </c>
+      <c r="N82" s="2">
+        <v>0</v>
+      </c>
+      <c r="O82" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB82" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="AC82" s="16">
+        <f t="shared" si="18"/>
+        <v>0.7</v>
+      </c>
+      <c r="AD82" s="18">
+        <f t="shared" si="19"/>
+        <v>0.2</v>
+      </c>
+      <c r="AE82" s="19">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF82" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG82" s="16">
+        <f t="shared" si="22"/>
+        <v>0.6</v>
+      </c>
+      <c r="AH82" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C83" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D83" s="3">
+        <v>8</v>
+      </c>
+      <c r="E83" s="2">
+        <v>2</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2">
+        <v>9</v>
+      </c>
+      <c r="H83" s="3">
+        <v>10</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2">
+        <v>0</v>
+      </c>
+      <c r="K83" s="2">
+        <v>10</v>
+      </c>
+      <c r="L83" s="3">
+        <v>3</v>
+      </c>
+      <c r="M83" s="2">
+        <v>7</v>
+      </c>
+      <c r="N83" s="2">
+        <v>0</v>
+      </c>
+      <c r="O83" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB83" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="AC83" s="16">
+        <f t="shared" si="18"/>
+        <v>0.8</v>
+      </c>
+      <c r="AD83" s="18">
+        <f t="shared" si="19"/>
+        <v>0.1</v>
+      </c>
+      <c r="AE83" s="19">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF83" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG83" s="16">
+        <f t="shared" si="22"/>
+        <v>0.3</v>
+      </c>
+      <c r="AH83" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C84" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="3">
+        <v>8</v>
+      </c>
+      <c r="E84" s="2">
+        <v>2</v>
+      </c>
+      <c r="F84" s="2">
+        <v>0</v>
+      </c>
+      <c r="G84" s="2">
+        <v>10</v>
+      </c>
+      <c r="H84" s="3">
+        <v>8</v>
+      </c>
+      <c r="I84" s="2">
+        <v>2</v>
+      </c>
+      <c r="J84" s="2">
+        <v>0</v>
+      </c>
+      <c r="K84" s="2">
+        <v>10</v>
+      </c>
+      <c r="L84" s="3">
+        <v>0</v>
+      </c>
+      <c r="M84" s="2">
+        <v>10</v>
+      </c>
+      <c r="N84" s="2">
+        <v>0</v>
+      </c>
+      <c r="O84" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB84" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="AC84" s="16">
+        <f t="shared" si="18"/>
+        <v>0.8</v>
+      </c>
+      <c r="AD84" s="18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE84" s="19">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="AF84" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG84" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH84" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C85" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="D85" s="3">
+        <v>9</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2">
+        <v>0</v>
+      </c>
+      <c r="G85" s="2">
+        <v>10</v>
+      </c>
+      <c r="H85" s="3">
+        <v>8</v>
+      </c>
+      <c r="I85" s="2">
+        <v>2</v>
+      </c>
+      <c r="J85" s="2">
+        <v>0</v>
+      </c>
+      <c r="K85" s="2">
+        <v>10</v>
+      </c>
+      <c r="L85" s="3">
+        <v>0</v>
+      </c>
+      <c r="M85" s="2">
+        <v>10</v>
+      </c>
+      <c r="N85" s="2">
+        <v>0</v>
+      </c>
+      <c r="O85" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB85" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="AC85" s="16">
+        <f t="shared" si="18"/>
+        <v>0.9</v>
+      </c>
+      <c r="AD85" s="18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE85" s="19">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="AF85" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG85" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH85" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C86" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="D86" s="3">
+        <v>10</v>
+      </c>
+      <c r="E86" s="2">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2">
+        <v>0</v>
+      </c>
+      <c r="G86" s="2">
+        <v>10</v>
+      </c>
+      <c r="H86" s="3">
+        <v>7</v>
+      </c>
+      <c r="I86" s="2">
+        <v>3</v>
+      </c>
+      <c r="J86" s="2">
+        <v>0</v>
+      </c>
+      <c r="K86" s="2">
+        <v>10</v>
+      </c>
+      <c r="L86" s="3">
+        <v>0</v>
+      </c>
+      <c r="M86" s="2">
+        <v>10</v>
+      </c>
+      <c r="N86" s="2">
+        <v>0</v>
+      </c>
+      <c r="O86" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB86" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="AC86" s="16">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="AD86" s="18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE86" s="19">
+        <f t="shared" si="20"/>
+        <v>0.7</v>
+      </c>
+      <c r="AF86" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG86" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH86" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C87" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D87" s="3">
+        <v>9</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2">
+        <v>0</v>
+      </c>
+      <c r="G87" s="2">
+        <v>10</v>
+      </c>
+      <c r="H87" s="3">
+        <v>6</v>
+      </c>
+      <c r="I87" s="2">
+        <v>4</v>
+      </c>
+      <c r="J87" s="2">
+        <v>0</v>
+      </c>
+      <c r="K87" s="2">
+        <v>10</v>
+      </c>
+      <c r="L87" s="3">
+        <v>0</v>
+      </c>
+      <c r="M87" s="2">
+        <v>10</v>
+      </c>
+      <c r="N87" s="2">
+        <v>0</v>
+      </c>
+      <c r="O87" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB87" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="AC87" s="16">
+        <f t="shared" si="18"/>
+        <v>0.9</v>
+      </c>
+      <c r="AD87" s="18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE87" s="19">
+        <f t="shared" si="20"/>
+        <v>0.6</v>
+      </c>
+      <c r="AF87" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG87" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH87" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="C88" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="D88" s="3">
+        <v>6</v>
+      </c>
+      <c r="E88" s="2">
+        <v>4</v>
+      </c>
+      <c r="F88" s="2">
+        <v>0</v>
+      </c>
+      <c r="G88" s="2">
+        <v>10</v>
+      </c>
+      <c r="H88" s="3">
+        <v>2</v>
+      </c>
+      <c r="I88" s="2">
+        <v>8</v>
+      </c>
+      <c r="J88" s="2">
+        <v>0</v>
+      </c>
+      <c r="K88" s="2">
+        <v>10</v>
+      </c>
+      <c r="L88" s="3">
+        <v>0</v>
+      </c>
+      <c r="M88" s="2">
+        <v>10</v>
+      </c>
+      <c r="N88" s="2">
+        <v>0</v>
+      </c>
+      <c r="O88" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB88" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="AC88" s="16">
+        <f t="shared" si="18"/>
+        <v>0.6</v>
+      </c>
+      <c r="AD88" s="18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE88" s="19">
+        <f t="shared" si="20"/>
+        <v>0.2</v>
+      </c>
+      <c r="AF88" s="17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG88" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH88" s="18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="3:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="10">
+        <v>1</v>
+      </c>
+      <c r="D89" s="5">
+        <v>2</v>
+      </c>
+      <c r="E89" s="6">
+        <v>8</v>
+      </c>
+      <c r="F89" s="6">
+        <v>0</v>
+      </c>
+      <c r="G89" s="6">
+        <v>10</v>
+      </c>
+      <c r="H89" s="5">
+        <v>0</v>
+      </c>
+      <c r="I89" s="6">
+        <v>10</v>
+      </c>
+      <c r="J89" s="6">
+        <v>0</v>
+      </c>
+      <c r="K89" s="6">
+        <v>10</v>
+      </c>
+      <c r="L89" s="5">
+        <v>0</v>
+      </c>
+      <c r="M89" s="6">
+        <v>10</v>
+      </c>
+      <c r="N89" s="6">
+        <v>0</v>
+      </c>
+      <c r="O89" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB89" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC89" s="20">
+        <f t="shared" si="18"/>
+        <v>0.2</v>
+      </c>
+      <c r="AD89" s="21">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE89" s="22">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AF89" s="23">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG89" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH89" s="21">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="49">
+    <mergeCell ref="AG60:AH60"/>
+    <mergeCell ref="AE60:AF60"/>
+    <mergeCell ref="AC60:AD60"/>
+    <mergeCell ref="AB60:AB61"/>
+    <mergeCell ref="AB59:AH59"/>
+    <mergeCell ref="C59:O59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="L60:O60"/>
+    <mergeCell ref="AB77:AH77"/>
+    <mergeCell ref="AB78:AB79"/>
+    <mergeCell ref="AC78:AD78"/>
+    <mergeCell ref="AE78:AF78"/>
+    <mergeCell ref="AG78:AH78"/>
+    <mergeCell ref="C77:O77"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="L78:O78"/>
+    <mergeCell ref="AB9:AH9"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AB26:AB27"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AB25:AH25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="C9:O9"/>
+    <mergeCell ref="C25:O25"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="Q11:U13"/>
     <mergeCell ref="Q52:U56"/>
     <mergeCell ref="V28:Z33"/>
     <mergeCell ref="V34:Z39"/>
@@ -3109,34 +4883,6 @@
     <mergeCell ref="Q34:U39"/>
     <mergeCell ref="Q40:U45"/>
     <mergeCell ref="Q46:U51"/>
-    <mergeCell ref="C9:O9"/>
-    <mergeCell ref="C25:O25"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="Q11:U13"/>
-    <mergeCell ref="Q14:U16"/>
-    <mergeCell ref="Q17:U19"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="V11:Z13"/>
-    <mergeCell ref="V14:Z16"/>
-    <mergeCell ref="V17:Z19"/>
-    <mergeCell ref="Q20:U22"/>
-    <mergeCell ref="V20:Z22"/>
-    <mergeCell ref="AB26:AB27"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AB25:AH25"/>
-    <mergeCell ref="AB9:AH9"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>